<commit_message>
Fix 0x201 Byte Order
</commit_message>
<xml_diff>
--- a/0x200-Assembly/[ignore]/RegisterBreakdown.xlsx
+++ b/0x200-Assembly/[ignore]/RegisterBreakdown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Projects\Z0FCourse_ReverseEngineering\0x200-Assembly\[ignore]\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDCC7C0-AB1C-4E0E-B371-6DD76FCA8FE8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFD1467-327D-4C51-8892-D98CB9671459}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1875" yWindow="1305" windowWidth="21600" windowHeight="11505" xr2:uid="{7A7D026D-FDE5-4D9B-A6DA-E7702BA901F5}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11505" xr2:uid="{7A7D026D-FDE5-4D9B-A6DA-E7702BA901F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -143,6 +143,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -150,12 +156,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -484,66 +484,66 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="10">
+      <c r="B1" s="7">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7">
+        <v>1</v>
+      </c>
+      <c r="D1" s="7">
+        <v>2</v>
+      </c>
+      <c r="E1" s="7">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7">
+        <v>4</v>
+      </c>
+      <c r="G1" s="7">
+        <v>5</v>
+      </c>
+      <c r="H1" s="7">
+        <v>6</v>
+      </c>
+      <c r="I1" s="7">
         <v>7</v>
-      </c>
-      <c r="C1" s="10">
-        <v>6</v>
-      </c>
-      <c r="D1" s="10">
-        <v>5</v>
-      </c>
-      <c r="E1" s="10">
-        <v>4</v>
-      </c>
-      <c r="F1" s="10">
-        <v>3</v>
-      </c>
-      <c r="G1" s="10">
-        <v>2</v>
-      </c>
-      <c r="H1" s="10">
-        <v>1</v>
-      </c>
-      <c r="I1" s="10">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="7"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="8"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="10"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="9"/>
+      <c r="F3" s="11"/>
       <c r="G3" s="2"/>
       <c r="H3" s="5" t="s">
         <v>3</v>

</xml_diff>